<commit_message>
1.Change generate file name 2.Change default excel
</commit_message>
<xml_diff>
--- a/AST2500.xlsx
+++ b/AST2500.xlsx
@@ -1921,16 +1921,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="C227" sqref="C227"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.375" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="20.25" customWidth="1"/>
-    <col min="4" max="4" width="11.625" customWidth="1"/>
+    <col min="3" max="3" width="60.25" customWidth="1"/>
+    <col min="4" max="4" width="19.625" customWidth="1"/>
     <col min="5" max="5" width="13.25" customWidth="1"/>
     <col min="6" max="6" width="17.25" customWidth="1"/>
   </cols>

</xml_diff>